<commit_message>
liste outils et personnages
</commit_message>
<xml_diff>
--- a/Copie deliste_outils.xlsx
+++ b/Copie deliste_outils.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="158">
   <si>
     <t>Liste des outils</t>
   </si>
@@ -426,9 +426,6 @@
     <t>Projectilateur à Pepsi</t>
   </si>
   <si>
-    <t>RÉGULIER : Attention! Cette crème glacé</t>
-  </si>
-  <si>
     <t>LÉGENDAIRE : Attention! Ce lance barbotine est réputé pour donner les pires "gels de cerveau".</t>
   </si>
   <si>
@@ -508,6 +505,18 @@
   </si>
   <si>
     <t>RÉGULIER : Personne ne sait pourquoi, mais les toutous ont une terrible phobie des ballons de plage.</t>
+  </si>
+  <si>
+    <t>RARE : Imaginez vous une noix de coco projeté à haute vitesse. Il y a de quoi faire peur!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RARE : Saviez-vous que le nom scientifique de la banane (musa sapientum) signifit homme rusé? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RARE : Saviez-vous qu'un ananas prend 3 ans à pousser? </t>
+  </si>
+  <si>
+    <t>RÉGULIER : Saviez-vous qu'un américain moyen consomme environ 23 litres de crème glacée par année? Il y a dequoi rendre jaloux ces gourmants toutous!</t>
   </si>
 </sst>
 </file>
@@ -612,7 +621,7 @@
       <name val="Liberation Sans"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,6 +703,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,7 +810,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -823,14 +838,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7"/>
@@ -1166,7 +1182,7 @@
   <dimension ref="A1:K202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+      <selection activeCell="Q59" sqref="Q59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1180,19 +1196,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -1297,7 +1313,7 @@
         <f t="shared" si="1"/>
         <v>15.625</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1332,7 +1348,7 @@
         <f t="shared" si="1"/>
         <v>15.625</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="16" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1369,8 +1385,8 @@
         <f t="shared" si="1"/>
         <v>22.5</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>136</v>
+      <c r="K6" s="16" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -1406,8 +1422,8 @@
         <f t="shared" si="1"/>
         <v>22.5</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>137</v>
+      <c r="K7" s="16" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -1443,8 +1459,8 @@
         <f t="shared" si="1"/>
         <v>22.5</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>135</v>
+      <c r="K8" s="16" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -1478,8 +1494,8 @@
         <f t="shared" si="1"/>
         <v>22.5</v>
       </c>
-      <c r="K9" s="17" t="s">
-        <v>134</v>
+      <c r="K9" s="16" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -1513,7 +1529,7 @@
         <f t="shared" si="1"/>
         <v>25.6</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="16" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1548,8 +1564,8 @@
         <f t="shared" si="1"/>
         <v>32.4</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>154</v>
+      <c r="K11" s="16" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -1583,8 +1599,8 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="K12" s="17" t="s">
-        <v>138</v>
+      <c r="K12" s="16" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
@@ -1618,7 +1634,7 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="16" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1653,7 +1669,7 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="16" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1688,7 +1704,7 @@
         <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="16" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1723,8 +1739,8 @@
         <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
-      <c r="K16" s="17" t="s">
-        <v>130</v>
+      <c r="K16" s="16" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
@@ -1760,8 +1776,8 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="K17" s="20" t="s">
-        <v>142</v>
+      <c r="K17" s="19" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
@@ -1795,8 +1811,8 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="K18" s="17" t="s">
-        <v>151</v>
+      <c r="K18" s="16" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.15">
@@ -1830,8 +1846,8 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="K19" s="19" t="s">
-        <v>133</v>
+      <c r="K19" s="18" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
@@ -1865,7 +1881,7 @@
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="K20" s="16" t="s">
+      <c r="K20" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1902,7 +1918,7 @@
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="K21" s="20" t="s">
+      <c r="K21" s="19" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1938,7 +1954,7 @@
         <v>160</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
@@ -1972,8 +1988,8 @@
         <f t="shared" si="1"/>
         <v>202.5</v>
       </c>
-      <c r="K23" s="17" t="s">
-        <v>141</v>
+      <c r="K23" s="16" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
@@ -2007,7 +2023,7 @@
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="K24" s="20" t="s">
+      <c r="K24" s="19" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2044,7 +2060,7 @@
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="K25" s="16" t="s">
+      <c r="K25" s="21" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2079,8 +2095,8 @@
         <f t="shared" si="1"/>
         <v>360</v>
       </c>
-      <c r="K26" s="17" t="s">
-        <v>140</v>
+      <c r="K26" s="16" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
@@ -2116,7 +2132,7 @@
         <f t="shared" si="1"/>
         <v>360</v>
       </c>
-      <c r="K27" s="20" t="s">
+      <c r="K27" s="19" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2151,8 +2167,8 @@
         <f t="shared" si="1"/>
         <v>390.625</v>
       </c>
-      <c r="K28" s="17" t="s">
-        <v>152</v>
+      <c r="K28" s="16" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
@@ -2223,8 +2239,8 @@
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="K30" s="17" t="s">
-        <v>129</v>
+      <c r="K30" s="16" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.15">
@@ -2258,8 +2274,8 @@
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="K31" s="17" t="s">
-        <v>139</v>
+      <c r="K31" s="16" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
@@ -2295,7 +2311,7 @@
         <f>(G32^2)/10</f>
         <v>1210</v>
       </c>
-      <c r="K32" s="17" t="s">
+      <c r="K32" s="16" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2332,8 +2348,8 @@
         <f t="shared" ref="J33:J60" si="2">(G33^2)/10</f>
         <v>1000</v>
       </c>
-      <c r="K33" s="17" t="s">
-        <v>147</v>
+      <c r="K33" s="16" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.15">
@@ -2369,8 +2385,8 @@
         <f t="shared" si="2"/>
         <v>810</v>
       </c>
-      <c r="K34" s="17" t="s">
-        <v>148</v>
+      <c r="K34" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
@@ -2406,8 +2422,8 @@
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="K35" s="17" t="s">
-        <v>143</v>
+      <c r="K35" s="16" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.15">
@@ -2443,8 +2459,8 @@
         <f t="shared" si="2"/>
         <v>640</v>
       </c>
-      <c r="K36" s="17" t="s">
-        <v>132</v>
+      <c r="K36" s="16" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.15">
@@ -2480,8 +2496,8 @@
         <f t="shared" si="2"/>
         <v>640</v>
       </c>
-      <c r="K37" s="17" t="s">
-        <v>128</v>
+      <c r="K37" s="16" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.15">
@@ -2517,7 +2533,7 @@
         <f t="shared" si="2"/>
         <v>490</v>
       </c>
-      <c r="K38" s="17" t="s">
+      <c r="K38" s="16" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2554,8 +2570,8 @@
         <f t="shared" si="2"/>
         <v>490</v>
       </c>
-      <c r="K39" s="17" t="s">
-        <v>150</v>
+      <c r="K39" s="16" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.15">
@@ -2591,8 +2607,8 @@
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="K40" s="17" t="s">
-        <v>131</v>
+      <c r="K40" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.15">
@@ -2628,8 +2644,8 @@
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="K41" s="17" t="s">
-        <v>149</v>
+      <c r="K41" s="16" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.15">
@@ -2666,7 +2682,7 @@
         <v>250</v>
       </c>
       <c r="K42" s="16" t="s">
-        <v>92</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.15">
@@ -2703,7 +2719,7 @@
         <v>250</v>
       </c>
       <c r="K43" s="16" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.15">
@@ -2739,8 +2755,8 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="K44" s="17" t="s">
-        <v>145</v>
+      <c r="K44" s="16" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.15">
@@ -2776,7 +2792,7 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="K45" s="17" t="s">
+      <c r="K45" s="16" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2813,7 +2829,7 @@
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="K46" s="16" t="s">
+      <c r="K46" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2887,8 +2903,8 @@
         <f t="shared" si="2"/>
         <v>122.5</v>
       </c>
-      <c r="K48" s="17" t="s">
-        <v>144</v>
+      <c r="K48" s="16" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.15">
@@ -2924,7 +2940,7 @@
         <f t="shared" si="2"/>
         <v>122.5</v>
       </c>
-      <c r="K49" s="18" t="s">
+      <c r="K49" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2961,7 +2977,7 @@
         <f t="shared" si="2"/>
         <v>122.5</v>
       </c>
-      <c r="K50" s="18" t="s">
+      <c r="K50" s="17" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2998,7 +3014,7 @@
         <f t="shared" si="2"/>
         <v>122.5</v>
       </c>
-      <c r="K51" s="18" t="s">
+      <c r="K51" s="17" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3036,7 +3052,7 @@
         <v>90</v>
       </c>
       <c r="K52" s="16" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.15">
@@ -3072,7 +3088,7 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="K53" s="18" t="s">
+      <c r="K53" s="17" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3109,7 +3125,7 @@
         <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
-      <c r="K54" s="18" t="s">
+      <c r="K54" s="17" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3146,7 +3162,7 @@
         <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
-      <c r="K55" s="18" t="s">
+      <c r="K55" s="17" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3183,8 +3199,8 @@
         <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
-      <c r="K56" s="17" t="s">
-        <v>146</v>
+      <c r="K56" s="16" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.15">
@@ -3220,8 +3236,8 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="K57" s="17" t="s">
-        <v>153</v>
+      <c r="K57" s="16" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.15">
@@ -3257,7 +3273,7 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K58" s="16" t="s">
+      <c r="K58" s="15" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3294,7 +3310,7 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K59" s="16" t="s">
+      <c r="K59" s="15" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>